<commit_message>
change scope of controllers and beans from (not working?) "view" to session/request
</commit_message>
<xml_diff>
--- a/time-records/Wagner_Claudia_csaw9017.xlsx
+++ b/time-records/Wagner_Claudia_csaw9017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\time-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0873A0-AFB0-46D3-BC67-AEFFFC18179C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997AD273-D46A-4425-A43C-F134A87DE0D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -146,6 +146,21 @@
   <si>
     <t>UI-Informationsmessages</t>
   </si>
+  <si>
+    <t>Use Case User Selbstregistrierung</t>
+  </si>
+  <si>
+    <t>Use Case User Erzeugen durch Admin + Würfeldialog</t>
+  </si>
+  <si>
+    <t>Teilnahme an Workshop6 Testen</t>
+  </si>
+  <si>
+    <t>User-related Tests</t>
+  </si>
+  <si>
+    <t>Use Case User Editieren durch Admin</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -239,6 +254,7 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -556,10 +572,10 @@
   <dimension ref="A1:D1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1075,59 +1091,158 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="8">
+        <v>44299</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="8">
+        <v>44300</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="8">
+        <v>44300</v>
+      </c>
+      <c r="B39" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-      <c r="D40" s="3"/>
+      <c r="A40" s="8">
+        <v>44301</v>
+      </c>
+      <c r="B40" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="8">
+        <v>44305</v>
+      </c>
+      <c r="B41" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="8">
+        <v>44306</v>
+      </c>
+      <c r="B42" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="8">
+        <v>44306</v>
+      </c>
+      <c r="B43" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="8">
+        <v>44306</v>
+      </c>
+      <c r="B44" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="8">
+        <v>44307</v>
+      </c>
+      <c r="B45" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="8">
+        <v>44308</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="8"/>
-      <c r="B47" s="7"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="8">
+        <v>44309</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="8"/>

</xml_diff>